<commit_message>
new updated automation framework from stating project class
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="TestLoginLogout" sheetId="1" r:id="rId1"/>
+    <sheet name="OrangeTC1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>usename</t>
   </si>
@@ -24,10 +24,19 @@
     <t>password</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>manager</t>
+    <t>opensourcecms</t>
+  </si>
+  <si>
+    <t>Homepageurl</t>
+  </si>
+  <si>
+    <t>Loginpageurl</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>index.php</t>
   </si>
 </sst>
 </file>
@@ -359,28 +368,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>